<commit_message>
Formulario de flipbooks adaptado para enfoque lector
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/10_formato_asignacion_temas_multiple_v2.xlsx
+++ b/assets/formatos_cargue/10_formato_asignacion_temas_multiple_v2.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Cód. tema</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>Número de la unidad en la que va el tema dentro del programa</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>Número que indica el orden en el que debe aparecer el tema dentro del programa</t>
   </si>
 </sst>
 </file>
@@ -518,7 +527,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +554,9 @@
       <c r="C1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -562,6 +573,9 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -573,6 +587,9 @@
       <c r="C3" s="3">
         <v>2</v>
       </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -582,6 +599,9 @@
         <v>14</v>
       </c>
       <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
         <v>3</v>
       </c>
     </row>
@@ -594,10 +614,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E5:I9"/>
+  <dimension ref="E5:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E10" sqref="E10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +664,7 @@
         <v>94</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" ref="I7:I9" si="0">E7 &amp; ", " &amp; F7 &amp; "," &amp; G7 &amp; "," &amp; H7</f>
+        <f t="shared" ref="I7:I10" si="0">E7 &amp; ", " &amp; F7 &amp; "," &amp; G7 &amp; "," &amp; H7</f>
         <v>A, Id Programa,ID del programa al que se asigna el tema,94</v>
       </c>
     </row>
@@ -682,6 +702,24 @@
       <c r="I9" t="str">
         <f t="shared" si="0"/>
         <v>C, Unidad,Número de la unidad en la que va el tema dentro del programa,1</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>D, Orden,Número que indica el orden en el que debe aparecer el tema dentro del programa,1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>